<commit_message>
added insulation constraints and added insulation to investement and service costs
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_one_month_one_household_one_car.xlsx
+++ b/src/pv_optimizer_contracting/data_input_one_month_one_household_one_car.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\OneDrive\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C55E8D5-E11C-4795-B423-9513F88CD88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD34FE6-2C37-4695-A09A-61B1B70C21B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
@@ -3510,7 +3510,7 @@
   <dimension ref="A1:S745"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3695,7 +3695,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -3705,7 +3705,7 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="9" t="s">
         <v>1002</v>
       </c>
       <c r="F4" t="s">
@@ -8220,7 +8220,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
fixed error in max pv capacity
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_one_month_one_household_one_car.xlsx
+++ b/src/pv_optimizer_contracting/data_input_one_month_one_household_one_car.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\OneDrive\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD75F55F-5274-4FD8-B583-38B23720224B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F493030-64EC-4083-81CF-AA6FCA157D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="1004">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="1006">
   <si>
     <t>PV</t>
   </si>
@@ -3077,6 +3077,12 @@
   </si>
   <si>
     <t>Number of residents</t>
+  </si>
+  <si>
+    <t>Capacity Density PV</t>
+  </si>
+  <si>
+    <t>rho_PV [kWp/m²]</t>
   </si>
 </sst>
 </file>
@@ -7560,10 +7566,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7637,57 +7643,57 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>1004</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>1005</v>
       </c>
       <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>1.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C7">
-        <v>0.9</v>
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>1.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8">
-        <v>70</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10">
         <v>50</v>
@@ -7695,32 +7701,32 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
       </c>
       <c r="C12">
-        <v>0.8</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
+        <v>48</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="C13">
         <v>0.8</v>
@@ -7728,10 +7734,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>37</v>
       </c>
       <c r="C14">
         <v>0.8</v>
@@ -7739,21 +7745,21 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>1003</v>
+        <v>112</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -7761,126 +7767,126 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>1003</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="C18">
-        <v>100</v>
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0.2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C21">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C22">
-        <v>0.3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C23">
-        <v>0.85</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C24">
-        <v>1.1000000000000001</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
+      </c>
+      <c r="B25" t="s">
+        <v>91</v>
       </c>
       <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>0.75</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0.75</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -7888,12 +7894,23 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>113</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>22</v>
       </c>
     </row>

</xml_diff>